<commit_message>
Ocean Energy enable 3^4 12h scenarios
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/FragilityCurvesData/ProbabilityEachScenario.xlsx
+++ b/CreateDB_NC/InputData/FragilityCurvesData/ProbabilityEachScenario.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,26 +488,40 @@
         <v>2030</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8099999999999999</v>
+        <v>0.62</v>
       </c>
       <c r="C4" t="n">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="D4" t="n">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2035</v>
+        <v>2040</v>
       </c>
       <c r="B5" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2050</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.8099999999999999</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C6" t="n">
         <v>0.15</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D6" t="n">
         <v>0.04</v>
       </c>
     </row>

</xml_diff>